<commit_message>
quality assurance and script correction
</commit_message>
<xml_diff>
--- a/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
+++ b/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-fish-diet-isotope/fish-diet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEB3085-8717-7E41-8C46-0236DFA8F6C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948F7287-7BC7-034E-B8FD-65E13B9247CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="2" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="1" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="367">
   <si>
     <t>Cruise</t>
   </si>
@@ -1427,6 +1427,9 @@
   <si>
     <t>Questionable</t>
   </si>
+  <si>
+    <t>Missing data from fisheries datasets</t>
+  </si>
 </sst>
 </file>
 
@@ -88895,8 +88898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269705B7-DB6F-CA4E-AC53-B891847B83EE}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -89023,6 +89026,12 @@
       <c r="D7" s="6" t="s">
         <v>344</v>
       </c>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -89037,6 +89046,12 @@
       <c r="F8" t="s">
         <v>256</v>
       </c>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H8" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -89067,6 +89082,12 @@
       </c>
       <c r="F10" t="s">
         <v>307</v>
+      </c>
+      <c r="G10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H10" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -89249,7 +89270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450A43-7CE0-8C4D-80E9-CDBE5E6D7720}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
revisions for upload to EDI
</commit_message>
<xml_diff>
--- a/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
+++ b/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-fish-diet-isotope/fish-diet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948F7287-7BC7-034E-B8FD-65E13B9247CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD58E0B-85C1-E844-AEB8-24F599B295E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="1" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="2" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="368">
   <si>
     <t>Cruise</t>
   </si>
@@ -1430,6 +1430,9 @@
   <si>
     <t>Missing data from fisheries datasets</t>
   </si>
+  <si>
+    <t>Missing Value</t>
+  </si>
 </sst>
 </file>
 
@@ -88898,7 +88901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269705B7-DB6F-CA4E-AC53-B891847B83EE}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -89268,10 +89271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450A43-7CE0-8C4D-80E9-CDBE5E6D7720}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -89351,6 +89354,17 @@
       </c>
       <c r="C7" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inserting custom parent project node and accomodating for empty fish guts
</commit_message>
<xml_diff>
--- a/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
+++ b/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-fish-diet-isotope/fish-diet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD58E0B-85C1-E844-AEB8-24F599B295E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3CCB93-FC81-AF44-BE90-F2C579BB2D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="2" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14720" activeTab="1" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="370">
   <si>
     <t>Cruise</t>
   </si>
@@ -1353,12 +1353,6 @@
     <t>Scientific name of prey item</t>
   </si>
   <si>
-    <t>Taxonomic serial number of fish specimen</t>
-  </si>
-  <si>
-    <t>Taxonomic serial number of prey item</t>
-  </si>
-  <si>
     <t>Common name of fish specimen</t>
   </si>
   <si>
@@ -1433,6 +1427,18 @@
   <si>
     <t>Missing Value</t>
   </si>
+  <si>
+    <t>Taxonomic serial number of prey item with prefix urn:lsid:itis.gov:itis_tsn:</t>
+  </si>
+  <si>
+    <t>Taxonomic serial number of fish specimen with prefix urn:lsid:itis.gov:itis_tsn:</t>
+  </si>
+  <si>
+    <t>Empty fish gut</t>
+  </si>
+  <si>
+    <t>Fork length not measured</t>
+  </si>
 </sst>
 </file>
 
@@ -1505,7 +1511,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1514,6 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -88899,10 +88906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269705B7-DB6F-CA4E-AC53-B891847B83EE}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -88993,7 +89000,7 @@
         <v>318</v>
       </c>
       <c r="C5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D5" t="s">
         <v>252</v>
@@ -89010,7 +89017,7 @@
         <v>319</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
         <v>252</v>
@@ -89021,19 +89028,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G7" t="s">
         <v>243</v>
       </c>
       <c r="H7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -89053,7 +89060,7 @@
         <v>243</v>
       </c>
       <c r="H8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -89090,7 +89097,7 @@
         <v>243</v>
       </c>
       <c r="H10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -89104,7 +89111,7 @@
         <v>332</v>
       </c>
       <c r="D11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -89112,10 +89119,10 @@
         <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>252</v>
@@ -89132,7 +89139,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D13" t="s">
         <v>252</v>
@@ -89149,13 +89156,19 @@
         <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>252</v>
       </c>
       <c r="E14" t="s">
-        <v>345</v>
+        <v>343</v>
+      </c>
+      <c r="G14" t="s">
+        <v>243</v>
+      </c>
+      <c r="H14" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -89183,7 +89196,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>295</v>
       </c>
@@ -89194,41 +89207,47 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>296</v>
       </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>317</v>
       </c>
       <c r="C19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>315</v>
       </c>
       <c r="C20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G20">
+        <v>-9999</v>
+      </c>
+      <c r="H20" t="s">
+        <v>368</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>320</v>
       </c>
@@ -89238,19 +89257,31 @@
       <c r="D21" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G21">
+        <v>-9999</v>
+      </c>
+      <c r="H21" t="s">
+        <v>368</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>321</v>
       </c>
       <c r="C22" t="s">
-        <v>342</v>
+        <v>366</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G22">
+        <v>-9999</v>
+      </c>
+      <c r="H22" t="s">
+        <v>368</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>316</v>
       </c>
@@ -89263,6 +89294,9 @@
       <c r="E23" t="s">
         <v>253</v>
       </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -89273,7 +89307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450A43-7CE0-8C4D-80E9-CDBE5E6D7720}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -89281,13 +89315,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" t="s">
         <v>361</v>
-      </c>
-      <c r="C1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -89336,35 +89370,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s">
         <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -89428,7 +89462,7 @@
         <v>271</v>
       </c>
       <c r="D2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>287</v>
@@ -89457,7 +89491,7 @@
         <v>275</v>
       </c>
       <c r="D3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G3" t="s">
         <v>291</v>
@@ -89480,7 +89514,7 @@
         <v>278</v>
       </c>
       <c r="D4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G4" t="s">
         <v>291</v>
@@ -89503,7 +89537,7 @@
         <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G5" t="s">
         <v>291</v>
@@ -89526,7 +89560,7 @@
         <v>284</v>
       </c>
       <c r="D6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G6" t="s">
         <v>292</v>
@@ -89549,7 +89583,7 @@
         <v>286</v>
       </c>
       <c r="D7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>288</v>
@@ -89561,7 +89595,7 @@
         <v>292</v>
       </c>
       <c r="H7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I7" t="s">
         <v>299</v>
@@ -89575,7 +89609,7 @@
         <v>293</v>
       </c>
       <c r="D8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>294</v>
@@ -89592,28 +89626,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
         <v>280</v>
       </c>
       <c r="C9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I9" t="s">
         <v>299</v>
       </c>
       <c r="J9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to personnel and renamed R Markdown file
</commit_message>
<xml_diff>
--- a/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
+++ b/fish-diet/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-fish-diet-isotope/fish-diet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01565F4-84A7-9D45-99E6-7678E7617781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1BA3F8-33EF-3548-B2B5-71D14274A248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14720" activeTab="3" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="364">
   <si>
     <t>Cruise</t>
   </si>
@@ -1230,24 +1230,6 @@
     <t>OCE-1655686</t>
   </si>
   <si>
-    <t>OCE-1655687</t>
-  </si>
-  <si>
-    <t>OCE-1655688</t>
-  </si>
-  <si>
-    <t>OCE-1655689</t>
-  </si>
-  <si>
-    <t>OCE-1655690</t>
-  </si>
-  <si>
-    <t>OCE-1655691</t>
-  </si>
-  <si>
-    <t>OCE-1655692</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
@@ -1398,9 +1380,6 @@
     <t>metadataProvider</t>
   </si>
   <si>
-    <t>OCE-1655693</t>
-  </si>
-  <si>
     <t>Northeast U.S. Shelf LTER</t>
   </si>
   <si>
@@ -1438,6 +1417,9 @@
   </si>
   <si>
     <t>principal investigator</t>
+  </si>
+  <si>
+    <t>0000-0001-9620-5382</t>
   </si>
 </sst>
 </file>
@@ -88952,10 +88934,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D2" t="s">
         <v>250</v>
@@ -88966,10 +88948,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D3" t="s">
         <v>252</v>
@@ -88983,10 +88965,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D4" t="s">
         <v>250</v>
@@ -88997,10 +88979,10 @@
         <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C5" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D5" t="s">
         <v>252</v>
@@ -89014,10 +88996,10 @@
         <v>242</v>
       </c>
       <c r="B6" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D6" t="s">
         <v>252</v>
@@ -89028,27 +89010,27 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C7" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G7" t="s">
         <v>243</v>
       </c>
       <c r="H7" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D8" t="s">
         <v>251</v>
@@ -89060,7 +89042,7 @@
         <v>243</v>
       </c>
       <c r="H8" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -89068,10 +89050,10 @@
         <v>244</v>
       </c>
       <c r="B9" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C9" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D9" t="s">
         <v>251</v>
@@ -89082,22 +89064,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C10" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D10" t="s">
         <v>251</v>
       </c>
       <c r="F10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G10" t="s">
         <v>243</v>
       </c>
       <c r="H10" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -89105,13 +89087,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C11" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -89119,10 +89101,10 @@
         <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C12" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>252</v>
@@ -89139,7 +89121,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D13" t="s">
         <v>252</v>
@@ -89153,22 +89135,22 @@
         <v>206</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C14" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>252</v>
       </c>
       <c r="E14" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G14" t="s">
         <v>243</v>
       </c>
       <c r="H14" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -89176,10 +89158,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C15" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D15" t="s">
         <v>250</v>
@@ -89187,10 +89169,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C16" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>250</v>
@@ -89201,7 +89183,7 @@
         <v>294</v>
       </c>
       <c r="C17" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>250</v>
@@ -89212,7 +89194,7 @@
         <v>295</v>
       </c>
       <c r="C18" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>250</v>
@@ -89220,10 +89202,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>250</v>
@@ -89232,10 +89214,10 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C20" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>250</v>
@@ -89244,15 +89226,15 @@
         <v>-9999</v>
       </c>
       <c r="H20" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C21" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>250</v>
@@ -89261,15 +89243,15 @@
         <v>-9999</v>
       </c>
       <c r="H21" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C22" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>250</v>
@@ -89278,15 +89260,15 @@
         <v>-9999</v>
       </c>
       <c r="H22" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C23" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>252</v>
@@ -89315,90 +89297,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="B1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B8" t="s">
         <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -89411,7 +89393,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -89462,7 +89444,7 @@
         <v>271</v>
       </c>
       <c r="D2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>287</v>
@@ -89491,7 +89473,7 @@
         <v>286</v>
       </c>
       <c r="D3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>288</v>
@@ -89500,16 +89482,16 @@
         <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="H3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="I3" t="s">
         <v>298</v>
       </c>
       <c r="J3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -89523,16 +89505,16 @@
         <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G4" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="I4" t="s">
         <v>298</v>
       </c>
       <c r="J4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -89546,7 +89528,7 @@
         <v>275</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G5" t="s">
         <v>291</v>
@@ -89555,7 +89537,7 @@
         <v>298</v>
       </c>
       <c r="J5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -89569,7 +89551,7 @@
         <v>278</v>
       </c>
       <c r="D6" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G6" t="s">
         <v>291</v>
@@ -89578,7 +89560,7 @@
         <v>298</v>
       </c>
       <c r="J6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -89592,7 +89574,7 @@
         <v>281</v>
       </c>
       <c r="D7" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G7" t="s">
         <v>291</v>
@@ -89601,7 +89583,7 @@
         <v>298</v>
       </c>
       <c r="J7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -89609,7 +89591,7 @@
         <v>292</v>
       </c>
       <c r="D8" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>293</v>
@@ -89621,33 +89603,36 @@
         <v>298</v>
       </c>
       <c r="J8" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B9" t="s">
         <v>280</v>
       </c>
       <c r="C9" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D9" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>352</v>
+        <v>346</v>
+      </c>
+      <c r="F9" t="s">
+        <v>363</v>
       </c>
       <c r="G9" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="I9" t="s">
         <v>298</v>
       </c>
       <c r="J9" t="s">
-        <v>356</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>